<commit_message>
geolocation field implemented, tested and documented
</commit_message>
<xml_diff>
--- a/formats/testdata/noformulas.xlsx
+++ b/formats/testdata/noformulas.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t xml:space="preserve">Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geopoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geopoint</t>
   </si>
   <si>
     <t xml:space="preserve">end repeat</t>
@@ -250,10 +256,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -396,46 +402,60 @@
       <c r="A13" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="B13" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="0" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="C16" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="C17" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -460,14 +480,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -478,35 +498,35 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
names must be identifiers
</commit_message>
<xml_diff>
--- a/formats/testdata/noformulas.xlsx
+++ b/formats/testdata/noformulas.xlsx
@@ -50,7 +50,7 @@
     <t xml:space="preserve">begin group</t>
   </si>
   <si>
-    <t xml:space="preserve">nested group</t>
+    <t xml:space="preserve">nested_group</t>
   </si>
   <si>
     <t xml:space="preserve">Nested Group</t>
@@ -113,7 +113,7 @@
     <t xml:space="preserve">end repeat</t>
   </si>
   <si>
-    <t xml:space="preserve">toplevel group</t>
+    <t xml:space="preserve">toplevel_group</t>
   </si>
   <si>
     <t xml:space="preserve">Toplevel Group</t>
@@ -122,7 +122,7 @@
     <t xml:space="preserve">select_one mealtime</t>
   </si>
   <si>
-    <t xml:space="preserve">single mealtime</t>
+    <t xml:space="preserve">single_mealtime</t>
   </si>
   <si>
     <t xml:space="preserve">Single Mealtime</t>
@@ -131,7 +131,7 @@
     <t xml:space="preserve">select_multiple mealtime</t>
   </si>
   <si>
-    <t xml:space="preserve">multiple mealtime</t>
+    <t xml:space="preserve">multiple_mealtime</t>
   </si>
   <si>
     <t xml:space="preserve">Multiple Mealtime</t>
@@ -259,16 +259,14 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,11 +476,10 @@
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added support for form tags/stringIdentifier
</commit_message>
<xml_diff>
--- a/formats/testdata/noformulas.xlsx
+++ b/formats/testdata/noformulas.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="choices" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="settings" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -165,6 +166,24 @@
   </si>
   <si>
     <t xml:space="preserve">Dinner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tag label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tag value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value2</t>
   </si>
 </sst>
 </file>
@@ -264,7 +283,7 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -551,4 +570,55 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added support for file and image fields
</commit_message>
<xml_diff>
--- a/formats/testdata/noformulas.xlsx
+++ b/formats/testdata/noformulas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t xml:space="preserve">Geopoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image</t>
   </si>
   <si>
     <t xml:space="preserve">end repeat</t>
@@ -281,10 +293,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -445,49 +457,71 @@
       <c r="A14" s="0" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -519,7 +553,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -530,35 +564,35 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -579,7 +613,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -590,26 +624,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new question type: textarea
</commit_message>
<xml_diff>
--- a/formats/testdata/noformulas.xlsx
+++ b/formats/testdata/noformulas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t xml:space="preserve">type some text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">textarea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Textarea</t>
   </si>
   <si>
     <t xml:space="preserve">end group</t>
@@ -293,10 +299,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -393,19 +399,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="B8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="0" t="s">
         <v>22</v>
       </c>
     </row>
@@ -431,7 +437,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>27</v>
       </c>
@@ -479,49 +485,60 @@
       <c r="A16" s="0" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="0" t="s">
+      <c r="B16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="C19" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="C20" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>43</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -553,7 +570,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -564,35 +581,35 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -624,26 +641,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
appearance:minimal for select questions
</commit_message>
<xml_diff>
--- a/formats/testdata/noformulas.xlsx
+++ b/formats/testdata/noformulas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -51,6 +51,9 @@
     <t xml:space="preserve">parameters</t>
   </si>
   <si>
+    <t xml:space="preserve">appearance</t>
+  </si>
+  <si>
     <t xml:space="preserve">begin repeat</t>
   </si>
   <si>
@@ -178,6 +181,9 @@
   </si>
   <si>
     <t xml:space="preserve">Single Mealtime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimal</t>
   </si>
   <si>
     <t xml:space="preserve">select_multiple mealtime</t>
@@ -326,10 +332,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -340,6 +346,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -370,16 +377,19 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>7</v>
@@ -387,222 +397,225 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -635,7 +648,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -646,35 +659,35 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -699,30 +712,30 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
textarea field replaced with text field with appearance:multiline
</commit_message>
<xml_diff>
--- a/formats/testdata/noformulas.xlsx
+++ b/formats/testdata/noformulas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t xml:space="preserve">Textarea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiline</t>
   </si>
   <si>
     <t xml:space="preserve">end group</t>
@@ -335,7 +338,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -467,7 +470,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>28</v>
@@ -478,103 +481,106 @@
       <c r="G9" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="J9" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -582,40 +588,40 @@
         <v>13</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -648,7 +654,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -659,35 +665,35 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -712,30 +718,30 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
formulas in groups readonly
</commit_message>
<xml_diff>
--- a/formats/testdata/noformulas.xlsx
+++ b/formats/testdata/noformulas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -344,7 +344,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -612,6 +612,9 @@
       </c>
       <c r="C22" s="0" t="s">
         <v>52</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>